<commit_message>
Tested another shunt & hall sensor, updated Readme
</commit_message>
<xml_diff>
--- a/Hall_Sensor/data/Hall_Sensoren.xlsx
+++ b/Hall_Sensor/data/Hall_Sensoren.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t xml:space="preserve">U_MM</t>
   </si>
@@ -43,10 +43,7 @@
     <t xml:space="preserve">A_Differenz</t>
   </si>
   <si>
-    <t xml:space="preserve">Prozent auf 4A – 20A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prozent auf 4A – 30A</t>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">ACS712</t>
@@ -67,6 +64,9 @@
     <t xml:space="preserve">30 A</t>
   </si>
   <si>
+    <t xml:space="preserve">5A</t>
+  </si>
+  <si>
     <t xml:space="preserve">5,006 V</t>
   </si>
   <si>
@@ -81,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -110,12 +110,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -166,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,16 +173,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -200,6 +190,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -210,14 +217,14 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X5" activeCellId="0" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="30.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,17 +272,27 @@
         <v>6</v>
       </c>
       <c r="P1" s="2"/>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
+      <c r="W1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
@@ -289,56 +306,70 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="V2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
@@ -365,7 +396,7 @@
         <f aca="false">C3-A3</f>
         <v>0.0369999999999999</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="2" t="n">
         <f aca="false">(A3-$A$30)/0.1</f>
         <v>-18.34</v>
       </c>
@@ -405,19 +436,32 @@
         <v>-0.848181818181818</v>
       </c>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="n">
-        <f aca="false">(G3/4)*100</f>
-        <v>-9.25000000000003</v>
-      </c>
-      <c r="R3" s="2" t="n">
-        <f aca="false">(O3/4)*100</f>
-        <v>-21.2045454545454</v>
-      </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
+      <c r="Q3" s="4" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="R3" s="4" t="n">
+        <v>-4.99</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <f aca="false">$Q$26+R3*0.185</f>
+        <v>1.56685</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <f aca="false">S3-Q3</f>
+        <v>1.08185</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <f aca="false">(Q3-$Q$26)/0.185</f>
+        <v>-10.8378378378378</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <f aca="false">(W3/5)*100</f>
+        <v>-116.956756756757</v>
+      </c>
+      <c r="W3" s="2" t="n">
+        <f aca="false">U3-R3</f>
+        <v>-5.84783783783784</v>
+      </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
@@ -444,7 +488,7 @@
         <f aca="false">C4-A4</f>
         <v>0.036</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="2" t="n">
         <f aca="false">(A4-$A$30)/0.1</f>
         <v>-17.34</v>
       </c>
@@ -484,19 +528,32 @@
         <v>-0.777575757575754</v>
       </c>
       <c r="P4" s="2"/>
-      <c r="Q4" s="2" t="n">
-        <f aca="false">(G4/4)*100</f>
-        <v>-8.99999999999999</v>
-      </c>
-      <c r="R4" s="2" t="n">
-        <f aca="false">(O4/4)*100</f>
-        <v>-19.4393939393938</v>
-      </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
+      <c r="Q4" s="4" t="n">
+        <v>0.525</v>
+      </c>
+      <c r="R4" s="4" t="n">
+        <v>-4.89</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <f aca="false">$Q$26+R4*0.185</f>
+        <v>1.58535</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <f aca="false">S4-Q4</f>
+        <v>1.06035</v>
+      </c>
+      <c r="U4" s="2" t="n">
+        <f aca="false">(Q4-$Q$26)/0.185</f>
+        <v>-10.6216216216216</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <f aca="false">(W4/5)*100</f>
+        <v>-114.632432432432</v>
+      </c>
+      <c r="W4" s="2" t="n">
+        <f aca="false">U4-R4</f>
+        <v>-5.73162162162162</v>
+      </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
@@ -523,7 +580,7 @@
         <f aca="false">C5-A5</f>
         <v>0.034</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="2" t="n">
         <f aca="false">(A5-$A$30)/0.1</f>
         <v>-16.33</v>
       </c>
@@ -563,19 +620,32 @@
         <v>-0.69181818181818</v>
       </c>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2" t="n">
-        <f aca="false">(G5/4)*100</f>
-        <v>-8.49999999999995</v>
-      </c>
-      <c r="R5" s="2" t="n">
-        <f aca="false">(O5/4)*100</f>
-        <v>-17.2954545454545</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
+      <c r="Q5" s="4" t="n">
+        <v>0.564</v>
+      </c>
+      <c r="R5" s="4" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <f aca="false">$Q$26+R5*0.185</f>
+        <v>1.602</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <f aca="false">S5-Q5</f>
+        <v>1.038</v>
+      </c>
+      <c r="U5" s="2" t="n">
+        <f aca="false">(Q5-$Q$26)/0.185</f>
+        <v>-10.4108108108108</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <f aca="false">(W5/5)*100</f>
+        <v>-112.216216216216</v>
+      </c>
+      <c r="W5" s="2" t="n">
+        <f aca="false">U5-R5</f>
+        <v>-5.61081081081081</v>
+      </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
@@ -602,7 +672,7 @@
         <f aca="false">C6-A6</f>
         <v>0.033</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="2" t="n">
         <f aca="false">(A6-$A$30)/0.1</f>
         <v>-15.32</v>
       </c>
@@ -642,19 +712,32 @@
         <v>-0.631212121212119</v>
       </c>
       <c r="P6" s="2"/>
-      <c r="Q6" s="2" t="n">
-        <f aca="false">(G6/4)*100</f>
-        <v>-8.25</v>
-      </c>
-      <c r="R6" s="2" t="n">
-        <f aca="false">(O6/4)*100</f>
-        <v>-15.780303030303</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
+      <c r="Q6" s="4" t="n">
+        <v>0.604</v>
+      </c>
+      <c r="R6" s="4" t="n">
+        <v>-4.69</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <f aca="false">$Q$26+R6*0.185</f>
+        <v>1.62235</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <f aca="false">S6-Q6</f>
+        <v>1.01835</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <f aca="false">(Q6-$Q$26)/0.185</f>
+        <v>-10.1945945945946</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <f aca="false">(W6/5)*100</f>
+        <v>-110.091891891892</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <f aca="false">U6-R6</f>
+        <v>-5.5045945945946</v>
+      </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
@@ -681,7 +764,7 @@
         <f aca="false">C7-A7</f>
         <v>0.0309999999999999</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="2" t="n">
         <f aca="false">(A7-$A$30)/0.1</f>
         <v>-14.31</v>
       </c>
@@ -721,19 +804,32 @@
         <v>-0.575757575757574</v>
       </c>
       <c r="P7" s="2"/>
-      <c r="Q7" s="2" t="n">
-        <f aca="false">(G7/4)*100</f>
-        <v>-7.75000000000001</v>
-      </c>
-      <c r="R7" s="2" t="n">
-        <f aca="false">(O7/4)*100</f>
-        <v>-14.3939393939394</v>
-      </c>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
+      <c r="Q7" s="4" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="R7" s="4" t="n">
+        <v>-4.6</v>
+      </c>
+      <c r="S7" s="2" t="n">
+        <f aca="false">$Q$26+R7*0.185</f>
+        <v>1.639</v>
+      </c>
+      <c r="T7" s="2" t="n">
+        <f aca="false">S7-Q7</f>
+        <v>0.995</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <f aca="false">(Q7-$Q$26)/0.185</f>
+        <v>-9.97837837837838</v>
+      </c>
+      <c r="V7" s="2" t="n">
+        <f aca="false">(W7/5)*100</f>
+        <v>-107.567567567568</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <f aca="false">U7-R7</f>
+        <v>-5.37837837837838</v>
+      </c>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
@@ -760,7 +856,7 @@
         <f aca="false">C8-A8</f>
         <v>0.03</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="2" t="n">
         <f aca="false">(A8-$A$30)/0.1</f>
         <v>-13.3</v>
       </c>
@@ -800,19 +896,32 @@
         <v>-0.530303030303029</v>
       </c>
       <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="n">
-        <f aca="false">(G8/4)*100</f>
-        <v>-7.50000000000002</v>
-      </c>
-      <c r="R8" s="2" t="n">
-        <f aca="false">(O8/4)*100</f>
-        <v>-13.2575757575757</v>
-      </c>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
+      <c r="Q8" s="4" t="n">
+        <v>0.684</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <f aca="false">$Q$26+R8*0.185</f>
+        <v>1.6575</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <f aca="false">S8-Q8</f>
+        <v>0.9735</v>
+      </c>
+      <c r="U8" s="2" t="n">
+        <f aca="false">(Q8-$Q$26)/0.185</f>
+        <v>-9.76216216216216</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <f aca="false">(W8/5)*100</f>
+        <v>-105.243243243243</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <f aca="false">U8-R8</f>
+        <v>-5.26216216216216</v>
+      </c>
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
@@ -839,7 +948,7 @@
         <f aca="false">C9-A9</f>
         <v>0.0270000000000001</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="2" t="n">
         <f aca="false">(A9-$A$30)/0.1</f>
         <v>-12.28</v>
       </c>
@@ -879,19 +988,32 @@
         <v>-0.474848484848485</v>
       </c>
       <c r="P9" s="2"/>
-      <c r="Q9" s="2" t="n">
-        <f aca="false">(G9/4)*100</f>
-        <v>-6.75000000000003</v>
-      </c>
-      <c r="R9" s="2" t="n">
-        <f aca="false">(O9/4)*100</f>
-        <v>-11.8712121212121</v>
-      </c>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
+      <c r="Q9" s="4" t="n">
+        <v>0.724</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>-4.4</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <f aca="false">$Q$26+R9*0.185</f>
+        <v>1.676</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <f aca="false">S9-Q9</f>
+        <v>0.952</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <f aca="false">(Q9-$Q$26)/0.185</f>
+        <v>-9.54594594594595</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <f aca="false">(W9/5)*100</f>
+        <v>-102.918918918919</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <f aca="false">U9-R9</f>
+        <v>-5.14594594594595</v>
+      </c>
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
@@ -918,7 +1040,7 @@
         <f aca="false">C10-A10</f>
         <v>0.0249999999999999</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="2" t="n">
         <f aca="false">(A10-$A$30)/0.1</f>
         <v>-11.26</v>
       </c>
@@ -958,19 +1080,32 @@
         <v>-0.444545454545453</v>
       </c>
       <c r="P10" s="2"/>
-      <c r="Q10" s="2" t="n">
-        <f aca="false">(G10/4)*100</f>
-        <v>-6.25</v>
-      </c>
-      <c r="R10" s="2" t="n">
-        <f aca="false">(O10/4)*100</f>
-        <v>-11.1136363636363</v>
-      </c>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
+      <c r="Q10" s="4" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="R10" s="4" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="S10" s="2" t="n">
+        <f aca="false">$Q$26+R10*0.185</f>
+        <v>1.6945</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <f aca="false">S10-Q10</f>
+        <v>0.9305</v>
+      </c>
+      <c r="U10" s="2" t="n">
+        <f aca="false">(Q10-$Q$26)/0.185</f>
+        <v>-9.32972972972973</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <f aca="false">(W10/5)*100</f>
+        <v>-100.594594594595</v>
+      </c>
+      <c r="W10" s="2" t="n">
+        <f aca="false">U10-R10</f>
+        <v>-5.02972972972973</v>
+      </c>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
@@ -997,7 +1132,7 @@
         <f aca="false">C11-A11</f>
         <v>0.0229999999999999</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="2" t="n">
         <f aca="false">(A11-$A$30)/0.1</f>
         <v>-10.24</v>
       </c>
@@ -1037,19 +1172,32 @@
         <v>-0.39909090909091</v>
       </c>
       <c r="P11" s="2"/>
-      <c r="Q11" s="2" t="n">
-        <f aca="false">(G11/4)*100</f>
-        <v>-5.75000000000001</v>
-      </c>
-      <c r="R11" s="2" t="n">
-        <f aca="false">(O11/4)*100</f>
-        <v>-9.97727272727276</v>
-      </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
+      <c r="Q11" s="4" t="n">
+        <v>0.804</v>
+      </c>
+      <c r="R11" s="4" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="S11" s="2" t="n">
+        <f aca="false">$Q$26+R11*0.185</f>
+        <v>1.713</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <f aca="false">S11-Q11</f>
+        <v>0.909</v>
+      </c>
+      <c r="U11" s="2" t="n">
+        <f aca="false">(Q11-$Q$26)/0.185</f>
+        <v>-9.11351351351351</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <f aca="false">(W11/5)*100</f>
+        <v>-98.2702702702703</v>
+      </c>
+      <c r="W11" s="2" t="n">
+        <f aca="false">U11-R11</f>
+        <v>-4.91351351351351</v>
+      </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
@@ -1076,7 +1224,7 @@
         <f aca="false">C12-A12</f>
         <v>0.0210000000000001</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="2" t="n">
         <f aca="false">(A12-$A$30)/0.1</f>
         <v>-9.22</v>
       </c>
@@ -1116,19 +1264,32 @@
         <v>-0.353636363636362</v>
       </c>
       <c r="P12" s="2"/>
-      <c r="Q12" s="2" t="n">
-        <f aca="false">(G12/4)*100</f>
-        <v>-5.25000000000002</v>
-      </c>
-      <c r="R12" s="2" t="n">
-        <f aca="false">(O12/4)*100</f>
-        <v>-8.84090909090904</v>
-      </c>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
+      <c r="Q12" s="4" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="R12" s="4" t="n">
+        <v>-4.1</v>
+      </c>
+      <c r="S12" s="2" t="n">
+        <f aca="false">$Q$26+R12*0.185</f>
+        <v>1.7315</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <f aca="false">S12-Q12</f>
+        <v>0.8875</v>
+      </c>
+      <c r="U12" s="2" t="n">
+        <f aca="false">(Q12-$Q$26)/0.185</f>
+        <v>-8.8972972972973</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <f aca="false">(W12/5)*100</f>
+        <v>-95.945945945946</v>
+      </c>
+      <c r="W12" s="2" t="n">
+        <f aca="false">U12-R12</f>
+        <v>-4.7972972972973</v>
+      </c>
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
@@ -1155,7 +1316,7 @@
         <f aca="false">C13-A13</f>
         <v>0.0189999999999999</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="2" t="n">
         <f aca="false">(A13-$A$30)/0.1</f>
         <v>-8.2</v>
       </c>
@@ -1195,19 +1356,32 @@
         <v>-0.323333333333334</v>
       </c>
       <c r="P13" s="2"/>
-      <c r="Q13" s="2" t="n">
-        <f aca="false">(G13/4)*100</f>
-        <v>-4.74999999999999</v>
-      </c>
-      <c r="R13" s="2" t="n">
-        <f aca="false">(O13/4)*100</f>
-        <v>-8.08333333333335</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
+      <c r="Q13" s="4" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>-3.99</v>
+      </c>
+      <c r="S13" s="2" t="n">
+        <f aca="false">$Q$26+R13*0.185</f>
+        <v>1.75185</v>
+      </c>
+      <c r="T13" s="2" t="n">
+        <f aca="false">S13-Q13</f>
+        <v>0.86885</v>
+      </c>
+      <c r="U13" s="2" t="n">
+        <f aca="false">(Q13-$Q$26)/0.185</f>
+        <v>-8.68648648648649</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <f aca="false">(W13/5)*100</f>
+        <v>-93.9297297297297</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <f aca="false">U13-R13</f>
+        <v>-4.69648648648649</v>
+      </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
@@ -1234,7 +1408,7 @@
         <f aca="false">C14-A14</f>
         <v>0.016</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="2" t="n">
         <f aca="false">(A14-$A$30)/0.1</f>
         <v>-7.17</v>
       </c>
@@ -1274,19 +1448,32 @@
         <v>-0.293030303030306</v>
       </c>
       <c r="P14" s="2"/>
-      <c r="Q14" s="2" t="n">
-        <f aca="false">(G14/4)*100</f>
-        <v>-4.00000000000003</v>
-      </c>
-      <c r="R14" s="2" t="n">
-        <f aca="false">(O14/4)*100</f>
-        <v>-7.32575757575764</v>
-      </c>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
+      <c r="Q14" s="4" t="n">
+        <v>1.284</v>
+      </c>
+      <c r="R14" s="4" t="n">
+        <v>-2.99</v>
+      </c>
+      <c r="S14" s="2" t="n">
+        <f aca="false">$Q$26+R14*0.185</f>
+        <v>1.93685</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <f aca="false">S14-Q14</f>
+        <v>0.65285</v>
+      </c>
+      <c r="U14" s="2" t="n">
+        <f aca="false">(Q14-$Q$26)/0.185</f>
+        <v>-6.51891891891892</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <f aca="false">(W14/5)*100</f>
+        <v>-70.5783783783784</v>
+      </c>
+      <c r="W14" s="2" t="n">
+        <f aca="false">U14-R14</f>
+        <v>-3.52891891891892</v>
+      </c>
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
@@ -1313,7 +1500,7 @@
         <f aca="false">C15-A15</f>
         <v>0.0150000000000001</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">(A15-$A$30)/0.1</f>
         <v>-6.15</v>
       </c>
@@ -1353,19 +1540,32 @@
         <v>-0.257575757575754</v>
       </c>
       <c r="P15" s="2"/>
-      <c r="Q15" s="2" t="n">
-        <f aca="false">(G15/4)*100</f>
-        <v>-3.75000000000005</v>
-      </c>
-      <c r="R15" s="2" t="n">
-        <f aca="false">(O15/4)*100</f>
-        <v>-6.43939393939386</v>
-      </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
+      <c r="Q15" s="4" t="n">
+        <v>1.684</v>
+      </c>
+      <c r="R15" s="4" t="n">
+        <v>-1.99</v>
+      </c>
+      <c r="S15" s="2" t="n">
+        <f aca="false">$Q$26+R15*0.185</f>
+        <v>2.12185</v>
+      </c>
+      <c r="T15" s="2" t="n">
+        <f aca="false">S15-Q15</f>
+        <v>0.43785</v>
+      </c>
+      <c r="U15" s="2" t="n">
+        <f aca="false">(Q15-$Q$26)/0.185</f>
+        <v>-4.35675675675676</v>
+      </c>
+      <c r="V15" s="2" t="n">
+        <f aca="false">(W15/5)*100</f>
+        <v>-47.3351351351352</v>
+      </c>
+      <c r="W15" s="2" t="n">
+        <f aca="false">U15-R15</f>
+        <v>-2.36675675675676</v>
+      </c>
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
@@ -1392,7 +1592,7 @@
         <f aca="false">C16-A16</f>
         <v>0.012</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">(A16-$A$30)/0.1</f>
         <v>-5.12</v>
       </c>
@@ -1432,19 +1632,32 @@
         <v>-0.22727272727273</v>
       </c>
       <c r="P16" s="2"/>
-      <c r="Q16" s="2" t="n">
-        <f aca="false">(G16/4)*100</f>
-        <v>-3</v>
-      </c>
-      <c r="R16" s="2" t="n">
-        <f aca="false">(O16/4)*100</f>
-        <v>-5.68181818181825</v>
-      </c>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
+      <c r="Q16" s="4" t="n">
+        <v>2.085</v>
+      </c>
+      <c r="R16" s="4" t="n">
+        <v>-0.99</v>
+      </c>
+      <c r="S16" s="2" t="n">
+        <f aca="false">$Q$26+R16*0.185</f>
+        <v>2.30685</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <f aca="false">S16-Q16</f>
+        <v>0.22185</v>
+      </c>
+      <c r="U16" s="2" t="n">
+        <f aca="false">(Q16-$Q$26)/0.185</f>
+        <v>-2.18918918918919</v>
+      </c>
+      <c r="V16" s="2" t="n">
+        <f aca="false">(W16/5)*100</f>
+        <v>-23.9837837837838</v>
+      </c>
+      <c r="W16" s="2" t="n">
+        <f aca="false">U16-R16</f>
+        <v>-1.19918918918919</v>
+      </c>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
@@ -1471,7 +1684,7 @@
         <f aca="false">C17-A17</f>
         <v>0.00900000000000034</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="2" t="n">
         <f aca="false">(A17-$A$30)/0.1</f>
         <v>-4.09</v>
       </c>
@@ -1511,19 +1724,32 @@
         <v>-0.181818181818179</v>
       </c>
       <c r="P17" s="2"/>
-      <c r="Q17" s="2" t="n">
-        <f aca="false">(G17/4)*100</f>
-        <v>-2.25000000000006</v>
-      </c>
-      <c r="R17" s="2" t="n">
-        <f aca="false">(O17/4)*100</f>
-        <v>-4.54545454545448</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
+      <c r="Q17" s="4" t="n">
+        <v>2.125</v>
+      </c>
+      <c r="R17" s="4" t="n">
+        <v>-0.89</v>
+      </c>
+      <c r="S17" s="2" t="n">
+        <f aca="false">$Q$26+R17*0.185</f>
+        <v>2.32535</v>
+      </c>
+      <c r="T17" s="2" t="n">
+        <f aca="false">S17-Q17</f>
+        <v>0.20035</v>
+      </c>
+      <c r="U17" s="2" t="n">
+        <f aca="false">(Q17-$Q$26)/0.185</f>
+        <v>-1.97297297297297</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <f aca="false">(W17/5)*100</f>
+        <v>-21.6594594594595</v>
+      </c>
+      <c r="W17" s="2" t="n">
+        <f aca="false">U17-R17</f>
+        <v>-1.08297297297297</v>
+      </c>
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
@@ -1550,7 +1776,7 @@
         <f aca="false">C18-A18</f>
         <v>0.00699999999999967</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" s="2" t="n">
         <f aca="false">(A18-$A$30)/0.1</f>
         <v>-3.07</v>
       </c>
@@ -1590,19 +1816,32 @@
         <v>-0.151515151515154</v>
       </c>
       <c r="P18" s="2"/>
-      <c r="Q18" s="2" t="n">
-        <f aca="false">(G18/4)*100</f>
-        <v>-1.74999999999999</v>
-      </c>
-      <c r="R18" s="2" t="n">
-        <f aca="false">(O18/4)*100</f>
-        <v>-3.78787878787885</v>
-      </c>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
+      <c r="Q18" s="4" t="n">
+        <v>2.166</v>
+      </c>
+      <c r="R18" s="4" t="n">
+        <v>-0.79</v>
+      </c>
+      <c r="S18" s="2" t="n">
+        <f aca="false">$Q$26+R18*0.185</f>
+        <v>2.34385</v>
+      </c>
+      <c r="T18" s="2" t="n">
+        <f aca="false">S18-Q18</f>
+        <v>0.17785</v>
+      </c>
+      <c r="U18" s="2" t="n">
+        <f aca="false">(Q18-$Q$26)/0.185</f>
+        <v>-1.75135135135135</v>
+      </c>
+      <c r="V18" s="2" t="n">
+        <f aca="false">(W18/5)*100</f>
+        <v>-19.2270270270271</v>
+      </c>
+      <c r="W18" s="2" t="n">
+        <f aca="false">U18-R18</f>
+        <v>-0.961351351351353</v>
+      </c>
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
@@ -1629,7 +1868,7 @@
         <f aca="false">C19-A19</f>
         <v>0.004</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="2" t="n">
         <f aca="false">(A19-$A$30)/0.1</f>
         <v>-2.04</v>
       </c>
@@ -1669,19 +1908,32 @@
         <v>-0.106060606060603</v>
       </c>
       <c r="P19" s="2"/>
-      <c r="Q19" s="2" t="n">
-        <f aca="false">(G19/4)*100</f>
-        <v>-1.00000000000005</v>
-      </c>
-      <c r="R19" s="2" t="n">
-        <f aca="false">(O19/4)*100</f>
-        <v>-2.65151515151507</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
+      <c r="Q19" s="4" t="n">
+        <v>2.206</v>
+      </c>
+      <c r="R19" s="4" t="n">
+        <v>-0.69</v>
+      </c>
+      <c r="S19" s="2" t="n">
+        <f aca="false">$Q$26+R19*0.185</f>
+        <v>2.36235</v>
+      </c>
+      <c r="T19" s="2" t="n">
+        <f aca="false">S19-Q19</f>
+        <v>0.15635</v>
+      </c>
+      <c r="U19" s="2" t="n">
+        <f aca="false">(Q19-$Q$26)/0.185</f>
+        <v>-1.53513513513514</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <f aca="false">(W19/5)*100</f>
+        <v>-16.9027027027027</v>
+      </c>
+      <c r="W19" s="2" t="n">
+        <f aca="false">U19-R19</f>
+        <v>-0.845135135135137</v>
+      </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
@@ -1708,7 +1960,7 @@
         <f aca="false">C20-A20</f>
         <v>0.00099999999999989</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="2" t="n">
         <f aca="false">(A20-$A$30)/0.1</f>
         <v>-1.01</v>
       </c>
@@ -1748,19 +2000,32 @@
         <v>-0.0606060606060581</v>
       </c>
       <c r="P20" s="2"/>
-      <c r="Q20" s="2" t="n">
-        <f aca="false">(G20/4)*100</f>
-        <v>-0.249999999999995</v>
-      </c>
-      <c r="R20" s="2" t="n">
-        <f aca="false">(O20/4)*100</f>
-        <v>-1.51515151515145</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="Q20" s="4" t="n">
+        <v>2.246</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>-0.59</v>
+      </c>
+      <c r="S20" s="2" t="n">
+        <f aca="false">$Q$26+R20*0.185</f>
+        <v>2.38085</v>
+      </c>
+      <c r="T20" s="2" t="n">
+        <f aca="false">S20-Q20</f>
+        <v>0.13485</v>
+      </c>
+      <c r="U20" s="2" t="n">
+        <f aca="false">(Q20-$Q$26)/0.185</f>
+        <v>-1.31891891891892</v>
+      </c>
+      <c r="V20" s="2" t="n">
+        <f aca="false">(W20/5)*100</f>
+        <v>-14.5783783783784</v>
+      </c>
+      <c r="W20" s="2" t="n">
+        <f aca="false">U20-R20</f>
+        <v>-0.72891891891892</v>
+      </c>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -1787,7 +2052,7 @@
         <f aca="false">C21-A21</f>
         <v>0.00099999999999989</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" s="2" t="n">
         <f aca="false">(A21-$A$30)/0.1</f>
         <v>-0.910000000000002</v>
       </c>
@@ -1827,19 +2092,32 @@
         <v>-0.054545454545457</v>
       </c>
       <c r="P21" s="2"/>
-      <c r="Q21" s="2" t="n">
-        <f aca="false">(G21/4)*100</f>
-        <v>-0.250000000000047</v>
-      </c>
-      <c r="R21" s="2" t="n">
-        <f aca="false">(O21/4)*100</f>
-        <v>-1.36363636363643</v>
-      </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
+      <c r="Q21" s="4" t="n">
+        <v>2.287</v>
+      </c>
+      <c r="R21" s="4" t="n">
+        <v>-0.49</v>
+      </c>
+      <c r="S21" s="2" t="n">
+        <f aca="false">$Q$26+R21*0.185</f>
+        <v>2.39935</v>
+      </c>
+      <c r="T21" s="2" t="n">
+        <f aca="false">S21-Q21</f>
+        <v>0.11235</v>
+      </c>
+      <c r="U21" s="2" t="n">
+        <f aca="false">(Q21-$Q$26)/0.185</f>
+        <v>-1.0972972972973</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <f aca="false">(W21/5)*100</f>
+        <v>-12.145945945946</v>
+      </c>
+      <c r="W21" s="2" t="n">
+        <f aca="false">U21-R21</f>
+        <v>-0.607297297297299</v>
+      </c>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
@@ -1866,7 +2144,7 @@
         <f aca="false">C22-A22</f>
         <v>0.00099999999999989</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" s="2" t="n">
         <f aca="false">(A22-$A$30)/0.1</f>
         <v>-0.81</v>
       </c>
@@ -1906,19 +2184,32 @@
         <v>-0.0484848484848491</v>
       </c>
       <c r="P22" s="2"/>
-      <c r="Q22" s="2" t="n">
-        <f aca="false">(G22/4)*100</f>
-        <v>-0.249999999999989</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <f aca="false">(O22/4)*100</f>
-        <v>-1.21212121212123</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
+      <c r="Q22" s="4" t="n">
+        <v>2.327</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="S22" s="2" t="n">
+        <f aca="false">$Q$26+R22*0.185</f>
+        <v>2.41785</v>
+      </c>
+      <c r="T22" s="2" t="n">
+        <f aca="false">S22-Q22</f>
+        <v>0.0908500000000001</v>
+      </c>
+      <c r="U22" s="2" t="n">
+        <f aca="false">(Q22-$Q$26)/0.185</f>
+        <v>-0.881081081081083</v>
+      </c>
+      <c r="V22" s="2" t="n">
+        <f aca="false">(W22/5)*100</f>
+        <v>-9.82162162162165</v>
+      </c>
+      <c r="W22" s="2" t="n">
+        <f aca="false">U22-R22</f>
+        <v>-0.491081081081083</v>
+      </c>
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
@@ -1945,7 +2236,7 @@
         <f aca="false">C23-A23</f>
         <v>0.00099999999999989</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" s="2" t="n">
         <f aca="false">(A23-$A$30)/0.1</f>
         <v>-0.710000000000002</v>
       </c>
@@ -1985,19 +2276,32 @@
         <v>-0.0424242424242414</v>
       </c>
       <c r="P23" s="2"/>
-      <c r="Q23" s="2" t="n">
-        <f aca="false">(G23/4)*100</f>
-        <v>-0.250000000000045</v>
-      </c>
-      <c r="R23" s="2" t="n">
-        <f aca="false">(O23/4)*100</f>
-        <v>-1.06060606060603</v>
-      </c>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+      <c r="Q23" s="4" t="n">
+        <v>2.368</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>-0.29</v>
+      </c>
+      <c r="S23" s="2" t="n">
+        <f aca="false">$Q$26+R23*0.185</f>
+        <v>2.43635</v>
+      </c>
+      <c r="T23" s="2" t="n">
+        <f aca="false">S23-Q23</f>
+        <v>0.0683500000000001</v>
+      </c>
+      <c r="U23" s="2" t="n">
+        <f aca="false">(Q23-$Q$26)/0.185</f>
+        <v>-0.659459459459461</v>
+      </c>
+      <c r="V23" s="2" t="n">
+        <f aca="false">(W23/5)*100</f>
+        <v>-7.38918918918923</v>
+      </c>
+      <c r="W23" s="2" t="n">
+        <f aca="false">U23-R23</f>
+        <v>-0.369459459459461</v>
+      </c>
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
@@ -2024,7 +2328,7 @@
         <f aca="false">C24-A24</f>
         <v>0</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="2" t="n">
         <f aca="false">(A24-$A$30)/0.1</f>
         <v>-0.600000000000001</v>
       </c>
@@ -2064,19 +2368,32 @@
         <v>-0.0363636363636336</v>
       </c>
       <c r="P24" s="2"/>
-      <c r="Q24" s="2" t="n">
-        <f aca="false">(G24/4)*100</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="2" t="n">
-        <f aca="false">(O24/4)*100</f>
-        <v>-0.90909090909084</v>
-      </c>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="Q24" s="4" t="n">
+        <v>2.408</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <v>-0.19</v>
+      </c>
+      <c r="S24" s="2" t="n">
+        <f aca="false">$Q$26+R24*0.185</f>
+        <v>2.45485</v>
+      </c>
+      <c r="T24" s="2" t="n">
+        <f aca="false">S24-Q24</f>
+        <v>0.0468500000000005</v>
+      </c>
+      <c r="U24" s="2" t="n">
+        <f aca="false">(Q24-$Q$26)/0.185</f>
+        <v>-0.443243243243245</v>
+      </c>
+      <c r="V24" s="2" t="n">
+        <f aca="false">(W24/5)*100</f>
+        <v>-5.0648648648649</v>
+      </c>
+      <c r="W24" s="2" t="n">
+        <f aca="false">U24-R24</f>
+        <v>-0.253243243243245</v>
+      </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
@@ -2103,7 +2420,7 @@
         <f aca="false">C25-A25</f>
         <v>0</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="2" t="n">
         <f aca="false">(A25-$A$30)/0.1</f>
         <v>-0.500000000000003</v>
       </c>
@@ -2143,19 +2460,32 @@
         <v>-0.0303030303030324</v>
       </c>
       <c r="P25" s="2"/>
-      <c r="Q25" s="2" t="n">
-        <f aca="false">(G25/4)*100</f>
-        <v>-6.66133814775094E-014</v>
-      </c>
-      <c r="R25" s="2" t="n">
-        <f aca="false">(O25/4)*100</f>
-        <v>-0.75757575757581</v>
-      </c>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
+      <c r="Q25" s="4" t="n">
+        <v>2.449</v>
+      </c>
+      <c r="R25" s="4" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="S25" s="2" t="n">
+        <f aca="false">$Q$26+R25*0.185</f>
+        <v>2.47335</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <f aca="false">S25-Q25</f>
+        <v>0.0243500000000005</v>
+      </c>
+      <c r="U25" s="2" t="n">
+        <f aca="false">(Q25-$Q$26)/0.185</f>
+        <v>-0.221621621621624</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <f aca="false">(W25/5)*100</f>
+        <v>-2.63243243243247</v>
+      </c>
+      <c r="W25" s="2" t="n">
+        <f aca="false">U25-R25</f>
+        <v>-0.131621621621624</v>
+      </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
@@ -2182,7 +2512,7 @@
         <f aca="false">C26-A26</f>
         <v>0</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" s="2" t="n">
         <f aca="false">(A26-$A$30)/0.1</f>
         <v>-0.4</v>
       </c>
@@ -2222,19 +2552,32 @@
         <v>-0.0242424242424246</v>
       </c>
       <c r="P26" s="2"/>
-      <c r="Q26" s="2" t="n">
-        <f aca="false">(G26/4)*100</f>
+      <c r="Q26" s="4" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="R26" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="R26" s="2" t="n">
-        <f aca="false">(O26/4)*100</f>
-        <v>-0.606060606060614</v>
-      </c>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
-      <c r="W26" s="2"/>
+      <c r="S26" s="2" t="n">
+        <f aca="false">$Q$26+R26*0.185</f>
+        <v>2.49</v>
+      </c>
+      <c r="T26" s="2" t="n">
+        <f aca="false">S26-Q26</f>
+        <v>0</v>
+      </c>
+      <c r="U26" s="2" t="n">
+        <f aca="false">(Q26-$Q$26)/0.185</f>
+        <v>0</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <f aca="false">(W26/5)*100</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="2" t="n">
+        <f aca="false">U26-R26</f>
+        <v>0</v>
+      </c>
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
@@ -2261,7 +2604,7 @@
         <f aca="false">C27-A27</f>
         <v>-0.00100000000000033</v>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" s="2" t="n">
         <f aca="false">(A27-$A$30)/0.1</f>
         <v>-0.289999999999999</v>
       </c>
@@ -2301,19 +2644,32 @@
         <v>-0.0333333333333303</v>
       </c>
       <c r="P27" s="2"/>
-      <c r="Q27" s="2" t="n">
-        <f aca="false">(G27/4)*100</f>
-        <v>0.250000000000021</v>
-      </c>
-      <c r="R27" s="2" t="n">
-        <f aca="false">(O27/4)*100</f>
-        <v>-0.833333333333257</v>
-      </c>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
+      <c r="Q27" s="4" t="n">
+        <v>2.528</v>
+      </c>
+      <c r="R27" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="S27" s="2" t="n">
+        <f aca="false">$Q$26+R27*0.185</f>
+        <v>2.5085</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <f aca="false">S27-Q27</f>
+        <v>-0.0194999999999999</v>
+      </c>
+      <c r="U27" s="2" t="n">
+        <f aca="false">(Q27-$Q$26)/0.185</f>
+        <v>0.205405405405404</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <f aca="false">(W27/5)*100</f>
+        <v>2.10810810810809</v>
+      </c>
+      <c r="W27" s="2" t="n">
+        <f aca="false">U27-R27</f>
+        <v>0.105405405405404</v>
+      </c>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
@@ -2340,7 +2696,7 @@
         <f aca="false">C28-A28</f>
         <v>-0.00099999999999989</v>
       </c>
-      <c r="E28" s="5" t="n">
+      <c r="E28" s="2" t="n">
         <f aca="false">(A28-$A$30)/0.1</f>
         <v>-0.190000000000001</v>
       </c>
@@ -2380,19 +2736,32 @@
         <v>-0.0272727272727291</v>
       </c>
       <c r="P28" s="2"/>
-      <c r="Q28" s="2" t="n">
-        <f aca="false">(G28/4)*100</f>
-        <v>0.249999999999968</v>
-      </c>
-      <c r="R28" s="2" t="n">
-        <f aca="false">(O28/4)*100</f>
-        <v>-0.681818181818229</v>
-      </c>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
+      <c r="Q28" s="4" t="n">
+        <v>2.568</v>
+      </c>
+      <c r="R28" s="4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="S28" s="2" t="n">
+        <f aca="false">$Q$26+R28*0.185</f>
+        <v>2.527</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <f aca="false">S28-Q28</f>
+        <v>-0.0409999999999999</v>
+      </c>
+      <c r="U28" s="2" t="n">
+        <f aca="false">(Q28-$Q$26)/0.185</f>
+        <v>0.421621621621621</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <f aca="false">(W28/5)*100</f>
+        <v>4.43243243243242</v>
+      </c>
+      <c r="W28" s="2" t="n">
+        <f aca="false">U28-R28</f>
+        <v>0.221621621621621</v>
+      </c>
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
@@ -2419,7 +2788,7 @@
         <f aca="false">C29-A29</f>
         <v>-0.00200000000000022</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" s="2" t="n">
         <f aca="false">(A29-$A$30)/0.1</f>
         <v>-0.0800000000000001</v>
       </c>
@@ -2459,19 +2828,32 @@
         <v>-0.0212121212121213</v>
       </c>
       <c r="P29" s="2"/>
-      <c r="Q29" s="2" t="n">
-        <f aca="false">(G29/4)*100</f>
-        <v>0.499999999999998</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <f aca="false">(O29/4)*100</f>
-        <v>-0.530303030303033</v>
-      </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
-      <c r="W29" s="2"/>
+      <c r="Q29" s="4" t="n">
+        <v>2.607</v>
+      </c>
+      <c r="R29" s="4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="S29" s="2" t="n">
+        <f aca="false">$Q$26+R29*0.185</f>
+        <v>2.5455</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <f aca="false">S29-Q29</f>
+        <v>-0.0615000000000001</v>
+      </c>
+      <c r="U29" s="2" t="n">
+        <f aca="false">(Q29-$Q$26)/0.185</f>
+        <v>0.632432432432432</v>
+      </c>
+      <c r="V29" s="2" t="n">
+        <f aca="false">(W29/5)*100</f>
+        <v>6.64864864864865</v>
+      </c>
+      <c r="W29" s="2" t="n">
+        <f aca="false">U29-R29</f>
+        <v>0.332432432432432</v>
+      </c>
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
@@ -2498,7 +2880,7 @@
         <f aca="false">C30-A30</f>
         <v>0</v>
       </c>
-      <c r="E30" s="5" t="n">
+      <c r="E30" s="2" t="n">
         <f aca="false">(A30-$A$30)/0.1</f>
         <v>0</v>
       </c>
@@ -2538,19 +2920,32 @@
         <v>0</v>
       </c>
       <c r="P30" s="2"/>
-      <c r="Q30" s="2" t="n">
-        <f aca="false">(G30/4)*100</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="2" t="n">
-        <f aca="false">(O30/4)*100</f>
-        <v>0</v>
-      </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
+      <c r="Q30" s="4" t="n">
+        <v>2.647</v>
+      </c>
+      <c r="R30" s="4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S30" s="2" t="n">
+        <f aca="false">$Q$26+R30*0.185</f>
+        <v>2.564</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <f aca="false">S30-Q30</f>
+        <v>-0.0829999999999997</v>
+      </c>
+      <c r="U30" s="2" t="n">
+        <f aca="false">(Q30-$Q$26)/0.185</f>
+        <v>0.848648648648646</v>
+      </c>
+      <c r="V30" s="2" t="n">
+        <f aca="false">(W30/5)*100</f>
+        <v>8.97297297297293</v>
+      </c>
+      <c r="W30" s="2" t="n">
+        <f aca="false">U30-R30</f>
+        <v>0.448648648648646</v>
+      </c>
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
@@ -2577,7 +2972,7 @@
         <f aca="false">C31-A31</f>
         <v>-0.00099999999999989</v>
       </c>
-      <c r="E31" s="5" t="n">
+      <c r="E31" s="2" t="n">
         <f aca="false">(A31-$A$30)/0.1</f>
         <v>0.109999999999997</v>
       </c>
@@ -2617,19 +3012,32 @@
         <v>0.00606060606060782</v>
       </c>
       <c r="P31" s="2"/>
-      <c r="Q31" s="2" t="n">
-        <f aca="false">(G31/4)*100</f>
-        <v>0.249999999999919</v>
-      </c>
-      <c r="R31" s="2" t="n">
-        <f aca="false">(O31/4)*100</f>
-        <v>0.151515151515196</v>
-      </c>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
+      <c r="Q31" s="4" t="n">
+        <v>2.688</v>
+      </c>
+      <c r="R31" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S31" s="2" t="n">
+        <f aca="false">$Q$26+R31*0.185</f>
+        <v>2.5825</v>
+      </c>
+      <c r="T31" s="2" t="n">
+        <f aca="false">S31-Q31</f>
+        <v>-0.1055</v>
+      </c>
+      <c r="U31" s="2" t="n">
+        <f aca="false">(Q31-$Q$26)/0.185</f>
+        <v>1.07027027027027</v>
+      </c>
+      <c r="V31" s="2" t="n">
+        <f aca="false">(W31/5)*100</f>
+        <v>11.4054054054054</v>
+      </c>
+      <c r="W31" s="2" t="n">
+        <f aca="false">U31-R31</f>
+        <v>0.57027027027027</v>
+      </c>
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
@@ -2656,7 +3064,7 @@
         <f aca="false">C32-A32</f>
         <v>-0.00099999999999989</v>
       </c>
-      <c r="E32" s="5" t="n">
+      <c r="E32" s="2" t="n">
         <f aca="false">(A32-$A$30)/0.1</f>
         <v>0.209999999999999</v>
       </c>
@@ -2696,19 +3104,32 @@
         <v>-0.00303030303030455</v>
       </c>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2" t="n">
-        <f aca="false">(G32/4)*100</f>
-        <v>0.249999999999977</v>
-      </c>
-      <c r="R32" s="2" t="n">
-        <f aca="false">(O32/4)*100</f>
-        <v>-0.0757575757576137</v>
-      </c>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
+      <c r="Q32" s="4" t="n">
+        <v>2.728</v>
+      </c>
+      <c r="R32" s="4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="S32" s="2" t="n">
+        <f aca="false">$Q$26+R32*0.185</f>
+        <v>2.601</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <f aca="false">S32-Q32</f>
+        <v>-0.127</v>
+      </c>
+      <c r="U32" s="2" t="n">
+        <f aca="false">(Q32-$Q$26)/0.185</f>
+        <v>1.28648648648649</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <f aca="false">(W32/5)*100</f>
+        <v>13.7297297297297</v>
+      </c>
+      <c r="W32" s="2" t="n">
+        <f aca="false">U32-R32</f>
+        <v>0.686486486486487</v>
+      </c>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
@@ -2735,7 +3156,7 @@
         <f aca="false">C33-A33</f>
         <v>-0.00200000000000022</v>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="2" t="n">
         <f aca="false">(A33-$A$30)/0.1</f>
         <v>0.32</v>
       </c>
@@ -2775,19 +3196,32 @@
         <v>-0.0121212121212102</v>
       </c>
       <c r="P33" s="2"/>
-      <c r="Q33" s="2" t="n">
-        <f aca="false">(G33/4)*100</f>
-        <v>0.500000000000007</v>
-      </c>
-      <c r="R33" s="2" t="n">
-        <f aca="false">(O33/4)*100</f>
-        <v>-0.303030303030255</v>
-      </c>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
+      <c r="Q33" s="4" t="n">
+        <v>2.768</v>
+      </c>
+      <c r="R33" s="4" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="S33" s="2" t="n">
+        <f aca="false">$Q$26+R33*0.185</f>
+        <v>2.6195</v>
+      </c>
+      <c r="T33" s="2" t="n">
+        <f aca="false">S33-Q33</f>
+        <v>-0.148499999999999</v>
+      </c>
+      <c r="U33" s="2" t="n">
+        <f aca="false">(Q33-$Q$26)/0.185</f>
+        <v>1.5027027027027</v>
+      </c>
+      <c r="V33" s="2" t="n">
+        <f aca="false">(W33/5)*100</f>
+        <v>16.054054054054</v>
+      </c>
+      <c r="W33" s="2" t="n">
+        <f aca="false">U33-R33</f>
+        <v>0.802702702702701</v>
+      </c>
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
@@ -2814,7 +3248,7 @@
         <f aca="false">C34-A34</f>
         <v>-0.00199999999999978</v>
       </c>
-      <c r="E34" s="5" t="n">
+      <c r="E34" s="2" t="n">
         <f aca="false">(A34-$A$30)/0.1</f>
         <v>0.419999999999998</v>
       </c>
@@ -2854,19 +3288,32 @@
         <v>-0.0060606060606091</v>
       </c>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2" t="n">
-        <f aca="false">(G34/4)*100</f>
-        <v>0.499999999999953</v>
-      </c>
-      <c r="R34" s="2" t="n">
-        <f aca="false">(O34/4)*100</f>
-        <v>-0.151515151515227</v>
-      </c>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="2"/>
+      <c r="Q34" s="4" t="n">
+        <v>2.808</v>
+      </c>
+      <c r="R34" s="4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <f aca="false">$Q$26+R34*0.185</f>
+        <v>2.638</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <f aca="false">S34-Q34</f>
+        <v>-0.169999999999999</v>
+      </c>
+      <c r="U34" s="2" t="n">
+        <f aca="false">(Q34-$Q$26)/0.185</f>
+        <v>1.71891891891892</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <f aca="false">(W34/5)*100</f>
+        <v>18.3783783783783</v>
+      </c>
+      <c r="W34" s="2" t="n">
+        <f aca="false">U34-R34</f>
+        <v>0.918918918918917</v>
+      </c>
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
@@ -2893,7 +3340,7 @@
         <f aca="false">C35-A35</f>
         <v>-0.012</v>
       </c>
-      <c r="E35" s="5" t="n">
+      <c r="E35" s="2" t="n">
         <f aca="false">(A35-$A$30)/0.1</f>
         <v>0.619999999999998</v>
       </c>
@@ -2933,19 +3380,32 @@
         <v>0</v>
       </c>
       <c r="P35" s="2"/>
-      <c r="Q35" s="2" t="n">
-        <f aca="false">(G35/4)*100</f>
-        <v>2.99999999999996</v>
-      </c>
-      <c r="R35" s="2" t="n">
-        <f aca="false">(O35/4)*100</f>
-        <v>0</v>
-      </c>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
+      <c r="Q35" s="4" t="n">
+        <v>2.848</v>
+      </c>
+      <c r="R35" s="4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="S35" s="2" t="n">
+        <f aca="false">$Q$26+R35*0.185</f>
+        <v>2.6565</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <f aca="false">S35-Q35</f>
+        <v>-0.1915</v>
+      </c>
+      <c r="U35" s="2" t="n">
+        <f aca="false">(Q35-$Q$26)/0.185</f>
+        <v>1.93513513513513</v>
+      </c>
+      <c r="V35" s="2" t="n">
+        <f aca="false">(W35/5)*100</f>
+        <v>20.7027027027027</v>
+      </c>
+      <c r="W35" s="2" t="n">
+        <f aca="false">U35-R35</f>
+        <v>1.03513513513513</v>
+      </c>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
@@ -2972,7 +3432,7 @@
         <f aca="false">C36-A36</f>
         <v>-0.00299999999999967</v>
       </c>
-      <c r="E36" s="5" t="n">
+      <c r="E36" s="2" t="n">
         <f aca="false">(A36-$A$30)/0.1</f>
         <v>0.629999999999997</v>
       </c>
@@ -3012,19 +3472,32 @@
         <v>0.00606060606060654</v>
       </c>
       <c r="P36" s="2"/>
-      <c r="Q36" s="2" t="n">
-        <f aca="false">(G36/4)*100</f>
-        <v>0.749999999999931</v>
-      </c>
-      <c r="R36" s="2" t="n">
-        <f aca="false">(O36/4)*100</f>
-        <v>0.151515151515164</v>
-      </c>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
+      <c r="Q36" s="4" t="n">
+        <v>2.888</v>
+      </c>
+      <c r="R36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="S36" s="2" t="n">
+        <f aca="false">$Q$26+R36*0.185</f>
+        <v>2.675</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <f aca="false">S36-Q36</f>
+        <v>-0.213</v>
+      </c>
+      <c r="U36" s="2" t="n">
+        <f aca="false">(Q36-$Q$26)/0.185</f>
+        <v>2.15135135135135</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <f aca="false">(W36/5)*100</f>
+        <v>23.027027027027</v>
+      </c>
+      <c r="W36" s="2" t="n">
+        <f aca="false">U36-R36</f>
+        <v>1.15135135135135</v>
+      </c>
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
@@ -3051,7 +3524,7 @@
         <f aca="false">C37-A37</f>
         <v>-0.00300000000000011</v>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E37" s="2" t="n">
         <f aca="false">(A37-$A$30)/0.1</f>
         <v>0.73</v>
       </c>
@@ -3091,19 +3564,32 @@
         <v>-0.00303030303030571</v>
       </c>
       <c r="P37" s="2"/>
-      <c r="Q37" s="2" t="n">
-        <f aca="false">(G37/4)*100</f>
-        <v>0.74999999999999</v>
-      </c>
-      <c r="R37" s="2" t="n">
-        <f aca="false">(O37/4)*100</f>
-        <v>-0.0757575757576429</v>
-      </c>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
+      <c r="Q37" s="4" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="R37" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S37" s="2" t="n">
+        <f aca="false">$Q$26+R37*0.185</f>
+        <v>2.86</v>
+      </c>
+      <c r="T37" s="2" t="n">
+        <f aca="false">S37-Q37</f>
+        <v>-0.43</v>
+      </c>
+      <c r="U37" s="2" t="n">
+        <f aca="false">(Q37-$Q$26)/0.185</f>
+        <v>4.32432432432432</v>
+      </c>
+      <c r="V37" s="2" t="n">
+        <f aca="false">(W37/5)*100</f>
+        <v>46.4864864864865</v>
+      </c>
+      <c r="W37" s="2" t="n">
+        <f aca="false">U37-R37</f>
+        <v>2.32432432432432</v>
+      </c>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
@@ -3130,7 +3616,7 @@
         <f aca="false">C38-A38</f>
         <v>-0.004</v>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="2" t="n">
         <f aca="false">(A38-$A$30)/0.1</f>
         <v>0.840000000000001</v>
       </c>
@@ -3170,19 +3656,32 @@
         <v>0.00303030303030194</v>
       </c>
       <c r="P38" s="2"/>
-      <c r="Q38" s="2" t="n">
-        <f aca="false">(G38/4)*100</f>
-        <v>1.00000000000002</v>
-      </c>
-      <c r="R38" s="2" t="n">
-        <f aca="false">(O38/4)*100</f>
-        <v>0.0757575757575485</v>
-      </c>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
+      <c r="Q38" s="4" t="n">
+        <v>3.692</v>
+      </c>
+      <c r="R38" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S38" s="2" t="n">
+        <f aca="false">$Q$26+R38*0.185</f>
+        <v>3.045</v>
+      </c>
+      <c r="T38" s="2" t="n">
+        <f aca="false">S38-Q38</f>
+        <v>-0.647</v>
+      </c>
+      <c r="U38" s="2" t="n">
+        <f aca="false">(Q38-$Q$26)/0.185</f>
+        <v>6.4972972972973</v>
+      </c>
+      <c r="V38" s="2" t="n">
+        <f aca="false">(W38/5)*100</f>
+        <v>69.945945945946</v>
+      </c>
+      <c r="W38" s="2" t="n">
+        <f aca="false">U38-R38</f>
+        <v>3.4972972972973</v>
+      </c>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
@@ -3209,7 +3708,7 @@
         <f aca="false">C39-A39</f>
         <v>-0.004</v>
       </c>
-      <c r="E39" s="5" t="n">
+      <c r="E39" s="2" t="n">
         <f aca="false">(A39-$A$30)/0.1</f>
         <v>0.939999999999999</v>
       </c>
@@ -3249,19 +3748,32 @@
         <v>0.00393939393939635</v>
       </c>
       <c r="P39" s="2"/>
-      <c r="Q39" s="2" t="n">
-        <f aca="false">(G39/4)*100</f>
-        <v>0.999999999999965</v>
-      </c>
-      <c r="R39" s="2" t="n">
-        <f aca="false">(O39/4)*100</f>
-        <v>0.0984848484849088</v>
-      </c>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
+      <c r="Q39" s="4" t="n">
+        <v>4.093</v>
+      </c>
+      <c r="R39" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S39" s="2" t="n">
+        <f aca="false">$Q$26+R39*0.185</f>
+        <v>3.23</v>
+      </c>
+      <c r="T39" s="2" t="n">
+        <f aca="false">S39-Q39</f>
+        <v>-0.863</v>
+      </c>
+      <c r="U39" s="2" t="n">
+        <f aca="false">(Q39-$Q$26)/0.185</f>
+        <v>8.66486486486486</v>
+      </c>
+      <c r="V39" s="2" t="n">
+        <f aca="false">(W39/5)*100</f>
+        <v>93.2972972972973</v>
+      </c>
+      <c r="W39" s="2" t="n">
+        <f aca="false">U39-R39</f>
+        <v>4.66486486486486</v>
+      </c>
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
@@ -3288,7 +3800,7 @@
         <f aca="false">C40-A40</f>
         <v>-0.0149999999999997</v>
       </c>
-      <c r="E40" s="5" t="n">
+      <c r="E40" s="2" t="n">
         <f aca="false">(A40-$A$30)/0.1</f>
         <v>1.15</v>
       </c>
@@ -3328,19 +3840,32 @@
         <v>0</v>
       </c>
       <c r="P40" s="2"/>
-      <c r="Q40" s="2" t="n">
-        <f aca="false">(G40/4)*100</f>
-        <v>3.74999999999994</v>
-      </c>
-      <c r="R40" s="2" t="n">
-        <f aca="false">(O40/4)*100</f>
-        <v>0</v>
-      </c>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
+      <c r="Q40" s="4" t="n">
+        <v>4.133</v>
+      </c>
+      <c r="R40" s="4" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="S40" s="2" t="n">
+        <f aca="false">$Q$26+R40*0.185</f>
+        <v>3.2485</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <f aca="false">S40-Q40</f>
+        <v>-0.8845</v>
+      </c>
+      <c r="U40" s="2" t="n">
+        <f aca="false">(Q40-$Q$26)/0.185</f>
+        <v>8.88108108108108</v>
+      </c>
+      <c r="V40" s="2" t="n">
+        <f aca="false">(W40/5)*100</f>
+        <v>95.6216216216216</v>
+      </c>
+      <c r="W40" s="2" t="n">
+        <f aca="false">U40-R40</f>
+        <v>4.78108108108108</v>
+      </c>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
@@ -3367,7 +3892,7 @@
         <f aca="false">C41-A41</f>
         <v>-0.02</v>
       </c>
-      <c r="E41" s="5" t="n">
+      <c r="E41" s="2" t="n">
         <f aca="false">(A41-$A$30)/0.1</f>
         <v>2.2</v>
       </c>
@@ -3407,19 +3932,32 @@
         <v>0.0151515151515151</v>
       </c>
       <c r="P41" s="2"/>
-      <c r="Q41" s="2" t="n">
-        <f aca="false">(G41/4)*100</f>
-        <v>4.99999999999994</v>
-      </c>
-      <c r="R41" s="2" t="n">
-        <f aca="false">(O41/4)*100</f>
-        <v>0.378787878787878</v>
-      </c>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="2"/>
+      <c r="Q41" s="4" t="n">
+        <v>4.173</v>
+      </c>
+      <c r="R41" s="4" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="S41" s="2" t="n">
+        <f aca="false">$Q$26+R41*0.185</f>
+        <v>3.267</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <f aca="false">S41-Q41</f>
+        <v>-0.906</v>
+      </c>
+      <c r="U41" s="2" t="n">
+        <f aca="false">(Q41-$Q$26)/0.185</f>
+        <v>9.0972972972973</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <f aca="false">(W41/5)*100</f>
+        <v>97.945945945946</v>
+      </c>
+      <c r="W41" s="2" t="n">
+        <f aca="false">U41-R41</f>
+        <v>4.8972972972973</v>
+      </c>
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
@@ -3446,7 +3984,7 @@
         <f aca="false">C42-A42</f>
         <v>-0.024</v>
       </c>
-      <c r="E42" s="5" t="n">
+      <c r="E42" s="2" t="n">
         <f aca="false">(A42-$A$30)/0.1</f>
         <v>3.24</v>
       </c>
@@ -3486,19 +4024,32 @@
         <v>0.0303030303030329</v>
       </c>
       <c r="P42" s="2"/>
-      <c r="Q42" s="2" t="n">
-        <f aca="false">(G42/4)*100</f>
-        <v>5.99999999999996</v>
-      </c>
-      <c r="R42" s="2" t="n">
-        <f aca="false">(O42/4)*100</f>
-        <v>0.757575757575824</v>
-      </c>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
-      <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
-      <c r="W42" s="2"/>
+      <c r="Q42" s="4" t="n">
+        <v>4.213</v>
+      </c>
+      <c r="R42" s="4" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="S42" s="2" t="n">
+        <f aca="false">$Q$26+R42*0.185</f>
+        <v>3.2855</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <f aca="false">S42-Q42</f>
+        <v>-0.9275</v>
+      </c>
+      <c r="U42" s="2" t="n">
+        <f aca="false">(Q42-$Q$26)/0.185</f>
+        <v>9.31351351351351</v>
+      </c>
+      <c r="V42" s="2" t="n">
+        <f aca="false">(W42/5)*100</f>
+        <v>100.27027027027</v>
+      </c>
+      <c r="W42" s="2" t="n">
+        <f aca="false">U42-R42</f>
+        <v>5.01351351351351</v>
+      </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
@@ -3525,7 +4076,7 @@
         <f aca="false">C43-A43</f>
         <v>-0.0289999999999999</v>
       </c>
-      <c r="E43" s="5" t="n">
+      <c r="E43" s="2" t="n">
         <f aca="false">(A43-$A$30)/0.1</f>
         <v>4.29</v>
       </c>
@@ -3565,19 +4116,32 @@
         <v>0.0454545454545441</v>
       </c>
       <c r="P43" s="2"/>
-      <c r="Q43" s="2" t="n">
-        <f aca="false">(G43/4)*100</f>
-        <v>7.24999999999996</v>
-      </c>
-      <c r="R43" s="2" t="n">
-        <f aca="false">(O43/4)*100</f>
-        <v>1.1363636363636</v>
-      </c>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
-      <c r="W43" s="2"/>
+      <c r="Q43" s="4" t="n">
+        <v>4.253</v>
+      </c>
+      <c r="R43" s="4" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="S43" s="2" t="n">
+        <f aca="false">$Q$26+R43*0.185</f>
+        <v>3.304</v>
+      </c>
+      <c r="T43" s="2" t="n">
+        <f aca="false">S43-Q43</f>
+        <v>-0.949</v>
+      </c>
+      <c r="U43" s="2" t="n">
+        <f aca="false">(Q43-$Q$26)/0.185</f>
+        <v>9.52972972972973</v>
+      </c>
+      <c r="V43" s="2" t="n">
+        <f aca="false">(W43/5)*100</f>
+        <v>102.594594594595</v>
+      </c>
+      <c r="W43" s="2" t="n">
+        <f aca="false">U43-R43</f>
+        <v>5.12972972972973</v>
+      </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
@@ -3604,7 +4168,7 @@
         <f aca="false">C44-A44</f>
         <v>-0.0339999999999998</v>
       </c>
-      <c r="E44" s="5" t="n">
+      <c r="E44" s="2" t="n">
         <f aca="false">(A44-$A$30)/0.1</f>
         <v>5.34</v>
       </c>
@@ -3644,19 +4208,32 @@
         <v>0.0757575757575753</v>
       </c>
       <c r="P44" s="2"/>
-      <c r="Q44" s="2" t="n">
-        <f aca="false">(G44/4)*100</f>
-        <v>8.49999999999995</v>
-      </c>
-      <c r="R44" s="2" t="n">
-        <f aca="false">(O44/4)*100</f>
-        <v>1.89393939393938</v>
-      </c>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
+      <c r="Q44" s="4" t="n">
+        <v>4.293</v>
+      </c>
+      <c r="R44" s="4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S44" s="2" t="n">
+        <f aca="false">$Q$26+R44*0.185</f>
+        <v>3.3225</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <f aca="false">S44-Q44</f>
+        <v>-0.9705</v>
+      </c>
+      <c r="U44" s="2" t="n">
+        <f aca="false">(Q44-$Q$26)/0.185</f>
+        <v>9.74594594594595</v>
+      </c>
+      <c r="V44" s="2" t="n">
+        <f aca="false">(W44/5)*100</f>
+        <v>104.918918918919</v>
+      </c>
+      <c r="W44" s="2" t="n">
+        <f aca="false">U44-R44</f>
+        <v>5.24594594594595</v>
+      </c>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
@@ -3683,7 +4260,7 @@
         <f aca="false">C45-A45</f>
         <v>-0.0379999999999998</v>
       </c>
-      <c r="E45" s="5" t="n">
+      <c r="E45" s="2" t="n">
         <f aca="false">(A45-$A$30)/0.1</f>
         <v>6.38</v>
       </c>
@@ -3723,19 +4300,32 @@
         <v>0.0909090909090926</v>
       </c>
       <c r="P45" s="2"/>
-      <c r="Q45" s="2" t="n">
-        <f aca="false">(G45/4)*100</f>
-        <v>9.49999999999998</v>
-      </c>
-      <c r="R45" s="2" t="n">
-        <f aca="false">(O45/4)*100</f>
-        <v>2.27272727272732</v>
-      </c>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
+      <c r="Q45" s="4" t="n">
+        <v>4.334</v>
+      </c>
+      <c r="R45" s="4" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="S45" s="2" t="n">
+        <f aca="false">$Q$26+R45*0.185</f>
+        <v>3.341</v>
+      </c>
+      <c r="T45" s="2" t="n">
+        <f aca="false">S45-Q45</f>
+        <v>-0.992999999999999</v>
+      </c>
+      <c r="U45" s="2" t="n">
+        <f aca="false">(Q45-$Q$26)/0.185</f>
+        <v>9.96756756756757</v>
+      </c>
+      <c r="V45" s="2" t="n">
+        <f aca="false">(W45/5)*100</f>
+        <v>107.351351351351</v>
+      </c>
+      <c r="W45" s="2" t="n">
+        <f aca="false">U45-R45</f>
+        <v>5.36756756756757</v>
+      </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
@@ -3762,7 +4352,7 @@
         <f aca="false">C46-A46</f>
         <v>-0.0419999999999998</v>
       </c>
-      <c r="E46" s="5" t="n">
+      <c r="E46" s="2" t="n">
         <f aca="false">(A46-$A$30)/0.1</f>
         <v>7.43</v>
       </c>
@@ -3802,19 +4392,32 @@
         <v>0.096060606060604</v>
       </c>
       <c r="P46" s="2"/>
-      <c r="Q46" s="2" t="n">
-        <f aca="false">(G46/4)*100</f>
-        <v>10.5</v>
-      </c>
-      <c r="R46" s="2" t="n">
-        <f aca="false">(O46/4)*100</f>
-        <v>2.4015151515151</v>
-      </c>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
+      <c r="Q46" s="4" t="n">
+        <v>4.372</v>
+      </c>
+      <c r="R46" s="4" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="S46" s="2" t="n">
+        <f aca="false">$Q$26+R46*0.185</f>
+        <v>3.3595</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <f aca="false">S46-Q46</f>
+        <v>-1.0125</v>
+      </c>
+      <c r="U46" s="2" t="n">
+        <f aca="false">(Q46-$Q$26)/0.185</f>
+        <v>10.172972972973</v>
+      </c>
+      <c r="V46" s="2" t="n">
+        <f aca="false">(W46/5)*100</f>
+        <v>109.459459459459</v>
+      </c>
+      <c r="W46" s="2" t="n">
+        <f aca="false">U46-R46</f>
+        <v>5.47297297297297</v>
+      </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
@@ -3841,7 +4444,7 @@
         <f aca="false">C47-A47</f>
         <v>-0.0450000000000004</v>
       </c>
-      <c r="E47" s="5" t="n">
+      <c r="E47" s="2" t="n">
         <f aca="false">(A47-$A$30)/0.1</f>
         <v>8.46</v>
       </c>
@@ -3881,19 +4484,32 @@
         <v>0.111212121212121</v>
       </c>
       <c r="P47" s="2"/>
-      <c r="Q47" s="2" t="n">
-        <f aca="false">(G47/4)*100</f>
-        <v>11.25</v>
-      </c>
-      <c r="R47" s="2" t="n">
-        <f aca="false">(O47/4)*100</f>
-        <v>2.78030303030303</v>
-      </c>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
+      <c r="Q47" s="4" t="n">
+        <v>4.414</v>
+      </c>
+      <c r="R47" s="4" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="S47" s="2" t="n">
+        <f aca="false">$Q$26+R47*0.185</f>
+        <v>3.378</v>
+      </c>
+      <c r="T47" s="2" t="n">
+        <f aca="false">S47-Q47</f>
+        <v>-1.036</v>
+      </c>
+      <c r="U47" s="2" t="n">
+        <f aca="false">(Q47-$Q$26)/0.185</f>
+        <v>10.4</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <f aca="false">(W47/5)*100</f>
+        <v>112</v>
+      </c>
+      <c r="W47" s="2" t="n">
+        <f aca="false">U47-R47</f>
+        <v>5.6</v>
+      </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
@@ -3920,7 +4536,7 @@
         <f aca="false">C48-A48</f>
         <v>-0.0489999999999999</v>
       </c>
-      <c r="E48" s="5" t="n">
+      <c r="E48" s="2" t="n">
         <f aca="false">(A48-$A$30)/0.1</f>
         <v>9.5</v>
       </c>
@@ -3960,19 +4576,32 @@
         <v>0.141515151515152</v>
       </c>
       <c r="P48" s="2"/>
-      <c r="Q48" s="2" t="n">
-        <f aca="false">(G48/4)*100</f>
-        <v>12.2499999999999</v>
-      </c>
-      <c r="R48" s="2" t="n">
-        <f aca="false">(O48/4)*100</f>
-        <v>3.53787878787881</v>
-      </c>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
+      <c r="Q48" s="4" t="n">
+        <v>4.455</v>
+      </c>
+      <c r="R48" s="4" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="S48" s="2" t="n">
+        <f aca="false">$Q$26+R48*0.185</f>
+        <v>3.3965</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <f aca="false">S48-Q48</f>
+        <v>-1.0585</v>
+      </c>
+      <c r="U48" s="2" t="n">
+        <f aca="false">(Q48-$Q$26)/0.185</f>
+        <v>10.6216216216216</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <f aca="false">(W48/5)*100</f>
+        <v>114.432432432432</v>
+      </c>
+      <c r="W48" s="2" t="n">
+        <f aca="false">U48-R48</f>
+        <v>5.72162162162162</v>
+      </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
@@ -3999,7 +4628,7 @@
         <f aca="false">C49-A49</f>
         <v>-0.0529999999999999</v>
       </c>
-      <c r="E49" s="5" t="n">
+      <c r="E49" s="2" t="n">
         <f aca="false">(A49-$A$30)/0.1</f>
         <v>10.54</v>
       </c>
@@ -4039,19 +4668,32 @@
         <v>0.171818181818184</v>
       </c>
       <c r="P49" s="2"/>
-      <c r="Q49" s="2" t="n">
-        <f aca="false">(G49/4)*100</f>
-        <v>13.2499999999999</v>
-      </c>
-      <c r="R49" s="2" t="n">
-        <f aca="false">(O49/4)*100</f>
-        <v>4.29545454545459</v>
-      </c>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
+      <c r="Q49" s="4" t="n">
+        <v>4.495</v>
+      </c>
+      <c r="R49" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S49" s="2" t="n">
+        <f aca="false">$Q$26+R49*0.185</f>
+        <v>3.415</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <f aca="false">S49-Q49</f>
+        <v>-1.08</v>
+      </c>
+      <c r="U49" s="2" t="n">
+        <f aca="false">(Q49-$Q$26)/0.185</f>
+        <v>10.8378378378378</v>
+      </c>
+      <c r="V49" s="2" t="n">
+        <f aca="false">(W49/5)*100</f>
+        <v>116.756756756757</v>
+      </c>
+      <c r="W49" s="2" t="n">
+        <f aca="false">U49-R49</f>
+        <v>5.83783783783784</v>
+      </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
@@ -4078,7 +4720,7 @@
         <f aca="false">C50-A50</f>
         <v>-0.0579999999999998</v>
       </c>
-      <c r="E50" s="5" t="n">
+      <c r="E50" s="2" t="n">
         <f aca="false">(A50-$A$30)/0.1</f>
         <v>11.59</v>
       </c>
@@ -4118,14 +4760,8 @@
         <v>0.186969696969696</v>
       </c>
       <c r="P50" s="2"/>
-      <c r="Q50" s="2" t="n">
-        <f aca="false">(G50/4)*100</f>
-        <v>14.5</v>
-      </c>
-      <c r="R50" s="2" t="n">
-        <f aca="false">(O50/4)*100</f>
-        <v>4.67424242424239</v>
-      </c>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -4157,7 +4793,7 @@
         <f aca="false">C51-A51</f>
         <v>-0.0619999999999998</v>
       </c>
-      <c r="E51" s="5" t="n">
+      <c r="E51" s="2" t="n">
         <f aca="false">(A51-$A$30)/0.1</f>
         <v>12.63</v>
       </c>
@@ -4197,14 +4833,8 @@
         <v>0.217272727272727</v>
       </c>
       <c r="P51" s="2"/>
-      <c r="Q51" s="2" t="n">
-        <f aca="false">(G51/4)*100</f>
-        <v>15.5</v>
-      </c>
-      <c r="R51" s="2" t="n">
-        <f aca="false">(O51/4)*100</f>
-        <v>5.43181818181817</v>
-      </c>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
@@ -4236,7 +4866,7 @@
         <f aca="false">C52-A52</f>
         <v>-0.0670000000000002</v>
       </c>
-      <c r="E52" s="5" t="n">
+      <c r="E52" s="2" t="n">
         <f aca="false">(A52-$A$30)/0.1</f>
         <v>13.67</v>
       </c>
@@ -4276,14 +4906,8 @@
         <v>0.257575757575758</v>
       </c>
       <c r="P52" s="2"/>
-      <c r="Q52" s="2" t="n">
-        <f aca="false">(G52/4)*100</f>
-        <v>16.75</v>
-      </c>
-      <c r="R52" s="2" t="n">
-        <f aca="false">(O52/4)*100</f>
-        <v>6.43939393939395</v>
-      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
@@ -4315,7 +4939,7 @@
         <f aca="false">C53-A53</f>
         <v>-0.0710000000000002</v>
       </c>
-      <c r="E53" s="5" t="n">
+      <c r="E53" s="2" t="n">
         <f aca="false">(A53-$A$30)/0.1</f>
         <v>14.71</v>
       </c>
@@ -4355,14 +4979,8 @@
         <v>0.287878787878789</v>
       </c>
       <c r="P53" s="2"/>
-      <c r="Q53" s="2" t="n">
-        <f aca="false">(G53/4)*100</f>
-        <v>17.75</v>
-      </c>
-      <c r="R53" s="2" t="n">
-        <f aca="false">(O53/4)*100</f>
-        <v>7.19696969696972</v>
-      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
@@ -4394,7 +5012,7 @@
         <f aca="false">C54-A54</f>
         <v>-0.077</v>
       </c>
-      <c r="E54" s="5" t="n">
+      <c r="E54" s="2" t="n">
         <f aca="false">(A54-$A$30)/0.1</f>
         <v>15.76</v>
       </c>
@@ -4434,14 +5052,8 @@
         <v>0.343333333333332</v>
       </c>
       <c r="P54" s="2"/>
-      <c r="Q54" s="2" t="n">
-        <f aca="false">(G54/4)*100</f>
-        <v>19.25</v>
-      </c>
-      <c r="R54" s="2" t="n">
-        <f aca="false">(O54/4)*100</f>
-        <v>8.5833333333333</v>
-      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
@@ -4473,7 +5085,7 @@
         <f aca="false">C55-A55</f>
         <v>-0.0810000000000004</v>
       </c>
-      <c r="E55" s="5" t="n">
+      <c r="E55" s="2" t="n">
         <f aca="false">(A55-$A$30)/0.1</f>
         <v>16.8</v>
       </c>
@@ -4513,14 +5125,8 @@
         <v>0.41909090909091</v>
       </c>
       <c r="P55" s="2"/>
-      <c r="Q55" s="2" t="n">
-        <f aca="false">(G55/4)*100</f>
-        <v>20.25</v>
-      </c>
-      <c r="R55" s="2" t="n">
-        <f aca="false">(O55/4)*100</f>
-        <v>10.4772727272727</v>
-      </c>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="2"/>
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
@@ -4552,7 +5158,7 @@
         <f aca="false">C56-A56</f>
         <v>-0.0860000000000003</v>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E56" s="2" t="n">
         <f aca="false">(A56-$A$30)/0.1</f>
         <v>17.84</v>
       </c>
@@ -4592,14 +5198,8 @@
         <v>0.459393939393934</v>
       </c>
       <c r="P56" s="2"/>
-      <c r="Q56" s="2" t="n">
-        <f aca="false">(G56/4)*100</f>
-        <v>21.5</v>
-      </c>
-      <c r="R56" s="2" t="n">
-        <f aca="false">(O56/4)*100</f>
-        <v>11.4848484848483</v>
-      </c>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
@@ -4631,7 +5231,7 @@
         <f aca="false">C57-A57</f>
         <v>-0.0919999999999996</v>
       </c>
-      <c r="E57" s="5" t="n">
+      <c r="E57" s="2" t="n">
         <f aca="false">(A57-$A$30)/0.1</f>
         <v>18.89</v>
       </c>
@@ -4671,14 +5271,8 @@
         <v>0.575454545454548</v>
       </c>
       <c r="P57" s="2"/>
-      <c r="Q57" s="2" t="n">
-        <f aca="false">(G57/4)*100</f>
-        <v>23</v>
-      </c>
-      <c r="R57" s="2" t="n">
-        <f aca="false">(O57/4)*100</f>
-        <v>14.3863636363637</v>
-      </c>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>

</xml_diff>